<commit_message>
Updated my gantt for the week
</commit_message>
<xml_diff>
--- a/Docs/Master_Gantt.xlsx
+++ b/Docs/Master_Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/walk5700_vandals_uidaho_edu/Documents/year 3/semester 1/cs383/git/CS-383-Project/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\CS-383-Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="353" documentId="8_{A9D32C3C-D3E6-499C-BAF4-A895A1CF4560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4073B46-0AA7-40FF-9DD5-0602D1F645FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E23EA-D1C7-4D56-85AF-94BCA5AC617D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="65">
   <si>
     <t>Total</t>
   </si>
@@ -147,27 +147,6 @@
     <t>Post Mortum Presentation Prep</t>
   </si>
   <si>
-    <t>Abby</t>
-  </si>
-  <si>
-    <t>Bill</t>
-  </si>
-  <si>
-    <t>Carley</t>
-  </si>
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>Erin</t>
-  </si>
-  <si>
-    <t>Fred</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
     <t>% Complete</t>
   </si>
   <si>
@@ -175,9 +154,6 @@
   </si>
   <si>
     <t>TL2: Austin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL1: </t>
   </si>
   <si>
     <t xml:space="preserve">TL3: </t>
@@ -204,9 +180,6 @@
     <t>Initial Platformer Planning</t>
   </si>
   <si>
-    <t>Nate</t>
-  </si>
-  <si>
     <t>Austin</t>
   </si>
   <si>
@@ -227,6 +200,39 @@
   <si>
     <t>SA Prep</t>
   </si>
+  <si>
+    <t>Godot Pong</t>
+  </si>
+  <si>
+    <t>Requirements Collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Design  </t>
+  </si>
+  <si>
+    <t>Level Difficultly Tables</t>
+  </si>
+  <si>
+    <t>Level Data Object design</t>
+  </si>
+  <si>
+    <t>User Documentation</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Installation</t>
+  </si>
+  <si>
+    <t>TL1: Nathan</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
 </sst>
 </file>
 
@@ -237,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,8 +350,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,8 +438,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="72">
+  <borders count="69">
     <border>
       <left/>
       <right/>
@@ -1098,51 +1155,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1294,11 +1306,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
@@ -1386,18 +1399,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="71" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1407,10 +1417,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1431,25 +1453,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1482,10 +1492,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -1868,46 +1890,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="17" width="12.7109375" customWidth="1"/>
+    <col min="3" max="17" width="12.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="94"/>
-      <c r="C2" s="91" t="s">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B2" s="91"/>
+      <c r="C2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="91" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="92"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="91" t="s">
+      <c r="G2" s="89"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="92"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="91" t="s">
+      <c r="J2" s="89"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="92"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="91" t="s">
+      <c r="M2" s="89"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="93"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="95"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="90"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="92"/>
       <c r="C3" s="76" t="s">
         <v>5</v>
       </c>
@@ -1954,33 +1976,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="79" t="s">
-        <v>36</v>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B4" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="C4" s="68">
         <f t="shared" ref="C4:D8" si="0">(F4+I4+L4+O4)</f>
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="D4" s="18">
         <f t="shared" si="0"/>
-        <v>1750</v>
+        <v>5650</v>
       </c>
       <c r="E4" s="67">
         <f t="shared" ref="E4:E8" si="1">(C4-D4)</f>
-        <v>4250</v>
+        <v>6350</v>
       </c>
       <c r="F4" s="66">
         <f>(Gantt!$B16)*100</f>
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="G4" s="23">
         <f>(Gantt!$C16)*100</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="H4" s="67">
         <f t="shared" ref="H4:H9" si="2">(F4-G4)</f>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="I4" s="68">
         <v>1000</v>
@@ -1995,31 +2017,31 @@
       </c>
       <c r="L4" s="68">
         <f>SA!C5*100</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="M4" s="18">
         <f>SA!D5*100</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N4" s="67">
         <f t="shared" ref="N4:N8" si="4">(L4-M4)</f>
-        <v>0</v>
+        <v>-300</v>
       </c>
       <c r="O4" s="68">
         <v>5000</v>
       </c>
       <c r="P4" s="18">
         <f>Overhead!B7*100</f>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="Q4" s="67">
         <f t="shared" ref="Q4:Q8" si="5">(O4-P4)</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="80" t="s">
-        <v>37</v>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B5" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C5" s="69">
         <f t="shared" si="0"/>
@@ -2080,33 +2102,33 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="68" t="e">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="68">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" s="18" t="e">
+        <v>6000</v>
+      </c>
+      <c r="D6" s="18">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E6" s="67" t="e">
+        <v>2800</v>
+      </c>
+      <c r="E6" s="67">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="F6" s="66" t="e">
-        <f>(Gantt!#REF!)*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G6" s="25" t="e">
-        <f>(Gantt!#REF!)*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H6" s="67" t="e">
+        <v>3200</v>
+      </c>
+      <c r="F6" s="66">
+        <f>(Gantt!$B46)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="25">
+        <f>(Gantt!$C46)*100</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="67">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="I6" s="68">
         <v>1000</v>
@@ -2143,9 +2165,9 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="80" t="s">
-        <v>39</v>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="B7" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C7" s="68">
         <f t="shared" si="0"/>
@@ -2206,33 +2228,33 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="68" t="e">
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="68">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="D8" s="18" t="e">
+        <v>6000</v>
+      </c>
+      <c r="D8" s="18">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E8" s="67" t="e">
+        <v>2350</v>
+      </c>
+      <c r="E8" s="67">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="F8" s="66" t="e">
-        <f>(Gantt!#REF!)*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G8" s="25" t="e">
-        <f>(Gantt!#REF!)*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H8" s="67" t="e">
+        <v>3650</v>
+      </c>
+      <c r="F8" s="66">
+        <f>(Gantt!$B61)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="66">
+        <f>(Gantt!$C61)*100</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="67">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="I8" s="68">
         <v>1000</v>
@@ -2269,33 +2291,33 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="70" t="e">
+      <c r="C9" s="70">
         <f>SUM(C4:C8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D9" s="71" t="e">
+        <v>37400</v>
+      </c>
+      <c r="D9" s="71">
         <f>SUM(D4:D8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E9" s="72" t="e">
+        <v>16400</v>
+      </c>
+      <c r="E9" s="72">
         <f>SUM(E4:E8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F9" s="73" t="e">
+        <v>21000</v>
+      </c>
+      <c r="F9" s="73">
         <f>SUM(F4:F8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G9" s="74" t="e">
+        <v>6000</v>
+      </c>
+      <c r="G9" s="74">
         <f>SUM(G4:G8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H9" s="72" t="e">
+        <v>3600</v>
+      </c>
+      <c r="H9" s="72">
         <f t="shared" si="2"/>
-        <v>#REF!</v>
+        <v>2400</v>
       </c>
       <c r="I9" s="70">
         <f t="shared" ref="I9:Q9" si="6">SUM(I4:I8)</f>
@@ -2311,15 +2333,15 @@
       </c>
       <c r="L9" s="70">
         <f t="shared" si="6"/>
-        <v>700</v>
+        <v>1400</v>
       </c>
       <c r="M9" s="70">
         <f t="shared" si="6"/>
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="N9" s="75">
         <f t="shared" si="6"/>
-        <v>200</v>
+        <v>-100</v>
       </c>
       <c r="O9" s="70">
         <f t="shared" si="6"/>
@@ -2327,41 +2349,41 @@
       </c>
       <c r="P9" s="70">
         <f t="shared" si="6"/>
-        <v>8100</v>
+        <v>8000</v>
       </c>
       <c r="Q9" s="75">
         <f t="shared" si="6"/>
-        <v>16900</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="F11" s="25"/>
       <c r="G11" s="23"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="F12" s="25"/>
       <c r="G12" s="24"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="F13" s="25" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2369,12 +2391,12 @@
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:8" x14ac:dyDescent="0.4">
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.4">
       <c r="F18" s="25"/>
       <c r="G18" s="23"/>
       <c r="H18" s="25"/>
@@ -2397,22 +2419,22 @@
   <dimension ref="A1:BE94"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3828125" bestFit="1" customWidth="1"/>
     <col min="7" max="54" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -2421,14 +2443,14 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="54" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -2487,14 +2509,14 @@
       <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
     </row>
-    <row r="2" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="103" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+    <row r="2" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="93" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="45">
         <v>1</v>
       </c>
@@ -2695,519 +2717,671 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50"/>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A3" s="116" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="116">
+        <v>1</v>
+      </c>
+      <c r="C3" s="116">
+        <v>1</v>
+      </c>
+      <c r="D3" s="124">
+        <v>1</v>
+      </c>
       <c r="E3" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="118"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="117"/>
+      <c r="AD3" s="117"/>
+      <c r="AE3" s="117"/>
+      <c r="AF3" s="117"/>
+      <c r="AG3" s="117"/>
+      <c r="AH3" s="117"/>
+      <c r="AI3" s="117"/>
+      <c r="AJ3" s="117"/>
+      <c r="AK3" s="117"/>
+      <c r="AL3" s="117"/>
+      <c r="AM3" s="117"/>
+      <c r="AN3" s="117"/>
+      <c r="AO3" s="117"/>
+      <c r="AP3" s="117"/>
+      <c r="AQ3" s="117"/>
+      <c r="AR3" s="117"/>
+      <c r="AS3" s="117"/>
+      <c r="AT3" s="117"/>
+      <c r="AU3" s="117"/>
+      <c r="AV3" s="117"/>
+      <c r="AW3" s="117"/>
+      <c r="AX3" s="117"/>
+      <c r="AY3" s="117"/>
+      <c r="AZ3" s="117"/>
+      <c r="BA3" s="117"/>
+      <c r="BB3" s="117"/>
+      <c r="BC3" s="117"/>
+      <c r="BD3" s="117"/>
+      <c r="BE3" s="117"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A4" s="116" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="116">
+        <v>3</v>
+      </c>
+      <c r="C4" s="116">
+        <v>3</v>
+      </c>
+      <c r="D4" s="125">
+        <v>1</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="117"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+      <c r="T4" s="119"/>
+      <c r="U4" s="119"/>
+      <c r="V4" s="119"/>
+      <c r="W4" s="119"/>
+      <c r="X4" s="119"/>
+      <c r="Y4" s="119"/>
+      <c r="Z4" s="119"/>
+      <c r="AA4" s="119"/>
+      <c r="AB4" s="119"/>
+      <c r="AC4" s="119"/>
+      <c r="AD4" s="119"/>
+      <c r="AE4" s="119"/>
+      <c r="AF4" s="119"/>
+      <c r="AG4" s="119"/>
+      <c r="AH4" s="119"/>
+      <c r="AI4" s="119"/>
+      <c r="AJ4" s="119"/>
+      <c r="AK4" s="119"/>
+      <c r="AL4" s="119"/>
+      <c r="AM4" s="119"/>
+      <c r="AN4" s="119"/>
+      <c r="AO4" s="119"/>
+      <c r="AP4" s="119"/>
+      <c r="AQ4" s="119"/>
+      <c r="AR4" s="119"/>
+      <c r="AS4" s="119"/>
+      <c r="AT4" s="119"/>
+      <c r="AU4" s="119"/>
+      <c r="AV4" s="119"/>
+      <c r="AW4" s="119"/>
+      <c r="AX4" s="119"/>
+      <c r="AY4" s="119"/>
+      <c r="AZ4" s="119"/>
+      <c r="BA4" s="119"/>
+      <c r="BB4" s="117"/>
+      <c r="BC4" s="117"/>
+      <c r="BD4" s="117"/>
+      <c r="BE4" s="117"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A5" s="116" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="120">
+        <v>10</v>
+      </c>
+      <c r="C5" s="120">
+        <v>8</v>
+      </c>
+      <c r="D5" s="125">
+        <v>1</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119"/>
+      <c r="T5" s="119"/>
+      <c r="U5" s="119"/>
+      <c r="V5" s="119"/>
+      <c r="W5" s="119"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="119"/>
+      <c r="Z5" s="119"/>
+      <c r="AA5" s="119"/>
+      <c r="AB5" s="119"/>
+      <c r="AC5" s="119"/>
+      <c r="AD5" s="119"/>
+      <c r="AE5" s="119"/>
+      <c r="AF5" s="119"/>
+      <c r="AG5" s="119"/>
+      <c r="AH5" s="119"/>
+      <c r="AI5" s="119"/>
+      <c r="AJ5" s="119"/>
+      <c r="AK5" s="119"/>
+      <c r="AL5" s="119"/>
+      <c r="AM5" s="119"/>
+      <c r="AN5" s="119"/>
+      <c r="AO5" s="119"/>
+      <c r="AP5" s="119"/>
+      <c r="AQ5" s="119"/>
+      <c r="AR5" s="119"/>
+      <c r="AS5" s="119"/>
+      <c r="AT5" s="119"/>
+      <c r="AU5" s="119"/>
+      <c r="AV5" s="119"/>
+      <c r="AW5" s="119"/>
+      <c r="AX5" s="119"/>
+      <c r="AY5" s="119"/>
+      <c r="AZ5" s="119"/>
+      <c r="BA5" s="119"/>
+      <c r="BB5" s="117"/>
+      <c r="BC5" s="117"/>
+      <c r="BD5" s="117"/>
+      <c r="BE5" s="117"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A6" s="116" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="120">
+        <v>10</v>
+      </c>
+      <c r="C6" s="120">
+        <v>8</v>
+      </c>
+      <c r="D6" s="125">
+        <v>1</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119"/>
+      <c r="Q6" s="119"/>
+      <c r="R6" s="118"/>
+      <c r="S6" s="118"/>
+      <c r="T6" s="118"/>
+      <c r="U6" s="118"/>
+      <c r="V6" s="118"/>
+      <c r="W6" s="118"/>
+      <c r="X6" s="118"/>
+      <c r="Y6" s="118"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="119"/>
+      <c r="AC6" s="119"/>
+      <c r="AD6" s="119"/>
+      <c r="AE6" s="119"/>
+      <c r="AF6" s="119"/>
+      <c r="AG6" s="119"/>
+      <c r="AH6" s="119"/>
+      <c r="AI6" s="119"/>
+      <c r="AJ6" s="119"/>
+      <c r="AK6" s="119"/>
+      <c r="AL6" s="119"/>
+      <c r="AM6" s="119"/>
+      <c r="AN6" s="119"/>
+      <c r="AO6" s="119"/>
+      <c r="AP6" s="119"/>
+      <c r="AQ6" s="119"/>
+      <c r="AR6" s="119"/>
+      <c r="AS6" s="119"/>
+      <c r="AT6" s="119"/>
+      <c r="AU6" s="119"/>
+      <c r="AV6" s="119"/>
+      <c r="AW6" s="119"/>
+      <c r="AX6" s="119"/>
+      <c r="AY6" s="119"/>
+      <c r="AZ6" s="117"/>
+      <c r="BA6" s="117"/>
+      <c r="BB6" s="117"/>
+      <c r="BC6" s="117"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A7" s="116" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="120">
+        <v>6</v>
+      </c>
+      <c r="C7" s="120">
+        <v>4</v>
+      </c>
+      <c r="D7" s="125">
+        <v>1</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="119"/>
+      <c r="Q7" s="119"/>
+      <c r="R7" s="119"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="119"/>
+      <c r="U7" s="119"/>
+      <c r="V7" s="119"/>
+      <c r="W7" s="119"/>
+      <c r="X7" s="119"/>
+      <c r="Y7" s="119"/>
+      <c r="Z7" s="117"/>
+      <c r="AA7" s="117"/>
+      <c r="AB7" s="118"/>
+      <c r="AC7" s="118"/>
+      <c r="AD7" s="118"/>
+      <c r="AE7" s="118"/>
+      <c r="AF7" s="118"/>
+      <c r="AG7" s="118"/>
+      <c r="AH7" s="119"/>
+      <c r="AI7" s="119"/>
+      <c r="AJ7" s="119"/>
+      <c r="AK7" s="119"/>
+      <c r="AL7" s="119"/>
+      <c r="AM7" s="119"/>
+      <c r="AN7" s="119"/>
+      <c r="AO7" s="119"/>
+      <c r="AP7" s="119"/>
+      <c r="AQ7" s="119"/>
+      <c r="AR7" s="119"/>
+      <c r="AS7" s="119"/>
+      <c r="AT7" s="119"/>
+      <c r="AU7" s="119"/>
+      <c r="AV7" s="119"/>
+      <c r="AW7" s="119"/>
+      <c r="AX7" s="119"/>
+      <c r="AY7" s="119"/>
+      <c r="AZ7" s="117"/>
+      <c r="BA7" s="117"/>
+      <c r="BB7" s="117"/>
+      <c r="BC7" s="117"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A8" s="116" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="120">
+        <v>2</v>
+      </c>
+      <c r="C8" s="120">
+        <v>2</v>
+      </c>
+      <c r="D8" s="125">
+        <v>1</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="117"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="119"/>
+      <c r="Q8" s="119"/>
+      <c r="R8" s="118"/>
+      <c r="S8" s="118"/>
+      <c r="T8" s="118"/>
+      <c r="U8" s="118"/>
+      <c r="V8" s="118"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="123"/>
+      <c r="Y8" s="123"/>
+      <c r="Z8" s="123"/>
+      <c r="AA8" s="123"/>
+      <c r="AB8" s="123"/>
+      <c r="AC8" s="123"/>
+      <c r="AD8" s="123"/>
+      <c r="AE8" s="123"/>
+      <c r="AF8" s="123"/>
+      <c r="AG8" s="123"/>
+      <c r="AH8" s="119"/>
+      <c r="AI8" s="119"/>
+      <c r="AJ8" s="119"/>
+      <c r="AK8" s="119"/>
+      <c r="AL8" s="119"/>
+      <c r="AM8" s="119"/>
+      <c r="AN8" s="119"/>
+      <c r="AO8" s="119"/>
+      <c r="AP8" s="119"/>
+      <c r="AQ8" s="119"/>
+      <c r="AR8" s="119"/>
+      <c r="AS8" s="119"/>
+      <c r="AT8" s="119"/>
+      <c r="AU8" s="119"/>
+      <c r="AV8" s="119"/>
+      <c r="AW8" s="119"/>
+      <c r="AX8" s="119"/>
+      <c r="AY8" s="119"/>
+      <c r="AZ8" s="117"/>
+      <c r="BA8" s="117"/>
+      <c r="BB8" s="117"/>
+      <c r="BC8" s="117"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A9" s="116" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="120">
+        <v>2</v>
+      </c>
+      <c r="C9" s="120">
+        <v>1</v>
+      </c>
+      <c r="D9" s="125">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="117"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
+      <c r="Q9" s="119"/>
+      <c r="R9" s="121"/>
+      <c r="S9" s="122"/>
+      <c r="T9" s="123"/>
+      <c r="U9" s="123"/>
+      <c r="V9" s="123"/>
+      <c r="W9" s="123"/>
+      <c r="X9" s="123"/>
+      <c r="Y9" s="123"/>
+      <c r="Z9" s="123"/>
+      <c r="AA9" s="123"/>
+      <c r="AB9" s="123"/>
+      <c r="AC9" s="123"/>
+      <c r="AD9" s="123"/>
+      <c r="AE9" s="123"/>
+      <c r="AF9" s="123"/>
+      <c r="AG9" s="123"/>
+      <c r="AH9" s="123"/>
+      <c r="AI9" s="123"/>
+      <c r="AJ9" s="123"/>
+      <c r="AK9" s="123"/>
+      <c r="AL9" s="123"/>
+      <c r="AM9" s="123"/>
+      <c r="AN9" s="123"/>
+      <c r="AO9" s="123"/>
+      <c r="AP9" s="123"/>
+      <c r="AQ9" s="123"/>
+      <c r="AR9" s="123"/>
+      <c r="AS9" s="123"/>
+      <c r="AT9" s="123"/>
+      <c r="AU9" s="123"/>
+      <c r="AV9" s="123"/>
+      <c r="AW9" s="123"/>
+      <c r="AX9" s="123"/>
+      <c r="AY9" s="123"/>
+      <c r="AZ9" s="117"/>
+      <c r="BA9" s="117"/>
+      <c r="BB9" s="117"/>
+      <c r="BC9" s="117"/>
+    </row>
+    <row r="10" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A10" s="116" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="120">
         <v>15</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-    </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="43"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="43"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="43"/>
-      <c r="AP4" s="43"/>
-      <c r="AQ4" s="43"/>
-      <c r="AR4" s="43"/>
-      <c r="AS4" s="43"/>
-      <c r="AT4" s="43"/>
-      <c r="AU4" s="43"/>
-      <c r="AV4" s="43"/>
-      <c r="AW4" s="43"/>
-      <c r="AX4" s="43"/>
-      <c r="AY4" s="43"/>
-      <c r="AZ4" s="43"/>
-      <c r="BA4" s="43"/>
-    </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="43"/>
-      <c r="AE5" s="43"/>
-      <c r="AF5" s="43"/>
-      <c r="AG5" s="43"/>
-      <c r="AH5" s="43"/>
-      <c r="AI5" s="43"/>
-      <c r="AJ5" s="43"/>
-      <c r="AK5" s="43"/>
-      <c r="AL5" s="43"/>
-      <c r="AM5" s="43"/>
-      <c r="AN5" s="43"/>
-      <c r="AO5" s="43"/>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="43"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="43"/>
-      <c r="AU5" s="43"/>
-      <c r="AV5" s="43"/>
-      <c r="AW5" s="43"/>
-      <c r="AX5" s="43"/>
-      <c r="AY5" s="43"/>
-      <c r="AZ5" s="43"/>
-      <c r="BA5" s="43"/>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="43"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="43"/>
-      <c r="AE6" s="43"/>
-      <c r="AF6" s="43"/>
-      <c r="AG6" s="43"/>
-      <c r="AH6" s="43"/>
-      <c r="AI6" s="43"/>
-      <c r="AJ6" s="43"/>
-      <c r="AK6" s="43"/>
-      <c r="AL6" s="43"/>
-      <c r="AM6" s="43"/>
-      <c r="AN6" s="43"/>
-      <c r="AO6" s="43"/>
-      <c r="AP6" s="43"/>
-      <c r="AQ6" s="43"/>
-      <c r="AR6" s="43"/>
-      <c r="AS6" s="43"/>
-      <c r="AT6" s="43"/>
-      <c r="AU6" s="43"/>
-      <c r="AV6" s="43"/>
-      <c r="AW6" s="43"/>
-      <c r="AX6" s="43"/>
-      <c r="AY6" s="43"/>
-      <c r="AZ6" s="43"/>
-      <c r="BA6" s="43"/>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="43"/>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="43"/>
-      <c r="AE7" s="43"/>
-      <c r="AF7" s="43"/>
-      <c r="AG7" s="43"/>
-      <c r="AH7" s="43"/>
-      <c r="AI7" s="43"/>
-      <c r="AJ7" s="43"/>
-      <c r="AK7" s="43"/>
-      <c r="AL7" s="43"/>
-      <c r="AM7" s="43"/>
-      <c r="AN7" s="43"/>
-      <c r="AO7" s="43"/>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="43"/>
-      <c r="AR7" s="43"/>
-      <c r="AS7" s="43"/>
-      <c r="AT7" s="43"/>
-      <c r="AU7" s="43"/>
-      <c r="AV7" s="43"/>
-      <c r="AW7" s="43"/>
-      <c r="AX7" s="43"/>
-      <c r="AY7" s="43"/>
-      <c r="AZ7" s="43"/>
-      <c r="BA7" s="43"/>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="43"/>
-      <c r="Z8" s="43"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="43"/>
-      <c r="AC8" s="43"/>
-      <c r="AD8" s="43"/>
-      <c r="AE8" s="43"/>
-      <c r="AF8" s="43"/>
-      <c r="AG8" s="43"/>
-      <c r="AH8" s="43"/>
-      <c r="AI8" s="43"/>
-      <c r="AJ8" s="43"/>
-      <c r="AK8" s="43"/>
-      <c r="AL8" s="43"/>
-      <c r="AM8" s="43"/>
-      <c r="AN8" s="43"/>
-      <c r="AO8" s="43"/>
-      <c r="AP8" s="43"/>
-      <c r="AQ8" s="43"/>
-      <c r="AR8" s="43"/>
-      <c r="AS8" s="43"/>
-      <c r="AT8" s="43"/>
-      <c r="AU8" s="43"/>
-      <c r="AV8" s="43"/>
-      <c r="AW8" s="43"/>
-      <c r="AX8" s="43"/>
-      <c r="AY8" s="43"/>
-      <c r="AZ8" s="43"/>
-      <c r="BA8" s="43"/>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="43"/>
-      <c r="AD9" s="43"/>
-      <c r="AE9" s="43"/>
-      <c r="AF9" s="43"/>
-      <c r="AG9" s="43"/>
-      <c r="AH9" s="43"/>
-      <c r="AI9" s="43"/>
-      <c r="AJ9" s="43"/>
-      <c r="AK9" s="43"/>
-      <c r="AL9" s="43"/>
-      <c r="AM9" s="43"/>
-      <c r="AN9" s="43"/>
-      <c r="AO9" s="43"/>
-      <c r="AP9" s="43"/>
-      <c r="AQ9" s="43"/>
-      <c r="AR9" s="43"/>
-      <c r="AS9" s="43"/>
-      <c r="AT9" s="43"/>
-      <c r="AU9" s="43"/>
-      <c r="AV9" s="43"/>
-      <c r="AW9" s="43"/>
-      <c r="AX9" s="43"/>
-      <c r="AY9" s="43"/>
-      <c r="AZ9" s="43"/>
-      <c r="BA9" s="43"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="52"/>
+      <c r="C10" s="120">
+        <v>3</v>
+      </c>
+      <c r="D10" s="125">
+        <v>0.2</v>
+      </c>
       <c r="E10" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="43"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="43"/>
-      <c r="AC10" s="43"/>
-      <c r="AD10" s="43"/>
-      <c r="AE10" s="43"/>
-      <c r="AF10" s="43"/>
-      <c r="AG10" s="43"/>
-      <c r="AH10" s="43"/>
-      <c r="AI10" s="43"/>
-      <c r="AJ10" s="43"/>
-      <c r="AK10" s="43"/>
-      <c r="AL10" s="43"/>
-      <c r="AM10" s="43"/>
-      <c r="AN10" s="43"/>
-      <c r="AO10" s="43"/>
-      <c r="AP10" s="43"/>
-      <c r="AQ10" s="43"/>
-      <c r="AR10" s="43"/>
-      <c r="AS10" s="43"/>
-      <c r="AT10" s="43"/>
-      <c r="AU10" s="43"/>
-      <c r="AV10" s="43"/>
-      <c r="AW10" s="43"/>
-      <c r="AX10" s="43"/>
-      <c r="AY10" s="43"/>
-      <c r="AZ10" s="43"/>
-      <c r="BA10" s="43"/>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
+        <v>14</v>
+      </c>
+      <c r="F10" s="117"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="119"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119"/>
+      <c r="T10" s="119"/>
+      <c r="U10" s="119"/>
+      <c r="V10" s="119"/>
+      <c r="W10" s="119"/>
+      <c r="X10" s="119"/>
+      <c r="Y10" s="119"/>
+      <c r="Z10" s="119"/>
+      <c r="AA10" s="119"/>
+      <c r="AB10" s="119"/>
+      <c r="AC10" s="119"/>
+      <c r="AD10" s="119"/>
+      <c r="AE10" s="119"/>
+      <c r="AF10" s="119"/>
+      <c r="AG10" s="119"/>
+      <c r="AH10" s="118"/>
+      <c r="AI10" s="118"/>
+      <c r="AJ10" s="118"/>
+      <c r="AK10" s="121"/>
+      <c r="AL10" s="121"/>
+      <c r="AM10" s="122"/>
+      <c r="AN10" s="122"/>
+      <c r="AO10" s="122"/>
+      <c r="AP10" s="122"/>
+      <c r="AQ10" s="122"/>
+      <c r="AR10" s="122"/>
+      <c r="AS10" s="122"/>
+      <c r="AT10" s="122"/>
+      <c r="AU10" s="122"/>
+      <c r="AV10" s="122"/>
+      <c r="AW10" s="119"/>
+      <c r="AX10" s="119"/>
+      <c r="AY10" s="119"/>
+      <c r="AZ10" s="119"/>
+      <c r="BA10" s="117"/>
+      <c r="BB10" s="117"/>
+      <c r="BC10" s="117"/>
+    </row>
+    <row r="11" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A11" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="120">
+        <v>3</v>
+      </c>
+      <c r="C11" s="120"/>
+      <c r="D11" s="125"/>
       <c r="E11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="43"/>
-      <c r="AD11" s="43"/>
-      <c r="AE11" s="43"/>
-      <c r="AF11" s="43"/>
-      <c r="AG11" s="43"/>
-      <c r="AH11" s="43"/>
-      <c r="AI11" s="43"/>
-      <c r="AJ11" s="43"/>
-      <c r="AK11" s="43"/>
-      <c r="AL11" s="43"/>
-      <c r="AM11" s="43"/>
-      <c r="AN11" s="43"/>
-      <c r="AO11" s="43"/>
-      <c r="AP11" s="43"/>
-      <c r="AQ11" s="43"/>
-      <c r="AR11" s="43"/>
-      <c r="AS11" s="43"/>
-      <c r="AT11" s="43"/>
-      <c r="AU11" s="43"/>
-      <c r="AV11" s="43"/>
-      <c r="AW11" s="43"/>
-      <c r="AX11" s="43"/>
-      <c r="AY11" s="43"/>
-      <c r="AZ11" s="43"/>
-      <c r="BA11" s="43"/>
-    </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="119"/>
+      <c r="Q11" s="119"/>
+      <c r="R11" s="119"/>
+      <c r="S11" s="119"/>
+      <c r="T11" s="119"/>
+      <c r="U11" s="119"/>
+      <c r="V11" s="119"/>
+      <c r="W11" s="119"/>
+      <c r="X11" s="119"/>
+      <c r="Y11" s="119"/>
+      <c r="Z11" s="119"/>
+      <c r="AA11" s="119"/>
+      <c r="AB11" s="119"/>
+      <c r="AC11" s="119"/>
+      <c r="AD11" s="119"/>
+      <c r="AE11" s="119"/>
+      <c r="AF11" s="119"/>
+      <c r="AG11" s="119"/>
+      <c r="AH11" s="119"/>
+      <c r="AI11" s="119"/>
+      <c r="AJ11" s="119"/>
+      <c r="AK11" s="119"/>
+      <c r="AL11" s="119"/>
+      <c r="AM11" s="119"/>
+      <c r="AN11" s="119"/>
+      <c r="AO11" s="119"/>
+      <c r="AP11" s="119"/>
+      <c r="AQ11" s="119"/>
+      <c r="AV11" s="119"/>
+      <c r="AW11" s="122"/>
+      <c r="AX11" s="122"/>
+      <c r="AY11" s="122"/>
+      <c r="AZ11" s="119"/>
+      <c r="BA11" s="117"/>
+      <c r="BB11" s="117"/>
+      <c r="BC11" s="117"/>
+    </row>
+    <row r="12" spans="1:57" x14ac:dyDescent="0.4">
+      <c r="A12" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="120">
+        <v>1</v>
+      </c>
+      <c r="C12" s="120"/>
+      <c r="D12" s="125"/>
       <c r="E12" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="43"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="43"/>
-      <c r="AF12" s="43"/>
-      <c r="AG12" s="43"/>
-      <c r="AH12" s="43"/>
-      <c r="AI12" s="43"/>
-      <c r="AJ12" s="43"/>
-      <c r="AK12" s="43"/>
-      <c r="AL12" s="43"/>
-      <c r="AM12" s="43"/>
-      <c r="AN12" s="43"/>
-      <c r="AO12" s="43"/>
-      <c r="AP12" s="43"/>
-      <c r="AQ12" s="43"/>
-      <c r="AR12" s="43"/>
-      <c r="AS12" s="43"/>
-      <c r="AT12" s="43"/>
-      <c r="AU12" s="43"/>
-      <c r="AV12" s="43"/>
-      <c r="AW12" s="43"/>
-      <c r="AX12" s="43"/>
-      <c r="AY12" s="43"/>
-      <c r="AZ12" s="43"/>
-      <c r="BA12" s="43"/>
-    </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="F12" s="117"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
+      <c r="Q12" s="119"/>
+      <c r="R12" s="119"/>
+      <c r="S12" s="119"/>
+      <c r="T12" s="119"/>
+      <c r="U12" s="119"/>
+      <c r="V12" s="119"/>
+      <c r="W12" s="119"/>
+      <c r="X12" s="119"/>
+      <c r="Y12" s="119"/>
+      <c r="Z12" s="119"/>
+      <c r="AA12" s="119"/>
+      <c r="AB12" s="119"/>
+      <c r="AC12" s="119"/>
+      <c r="AD12" s="119"/>
+      <c r="AE12" s="119"/>
+      <c r="AF12" s="119"/>
+      <c r="AG12" s="119"/>
+      <c r="AH12" s="119"/>
+      <c r="AI12" s="119"/>
+      <c r="AJ12" s="119"/>
+      <c r="AK12" s="119"/>
+      <c r="AL12" s="119"/>
+      <c r="AM12" s="119"/>
+      <c r="AN12" s="119"/>
+      <c r="AO12" s="119"/>
+      <c r="AP12" s="119"/>
+      <c r="AQ12" s="119"/>
+      <c r="AV12" s="119"/>
+      <c r="AW12" s="119"/>
+      <c r="AX12" s="119"/>
+      <c r="AY12" s="119"/>
+      <c r="AZ12" s="122"/>
+      <c r="BA12" s="117"/>
+      <c r="BB12" s="117"/>
+      <c r="BC12" s="117"/>
+    </row>
+    <row r="13" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A13" s="47"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
+      <c r="D13" s="126"/>
       <c r="E13" s="44" t="s">
         <v>15</v>
       </c>
@@ -3255,14 +3429,12 @@
       <c r="AW13" s="43"/>
       <c r="AX13" s="43"/>
       <c r="AY13" s="43"/>
-      <c r="AZ13" s="43"/>
-      <c r="BA13" s="43"/>
-    </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A14" s="47"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="D14" s="126"/>
       <c r="E14" s="44" t="s">
         <v>15</v>
       </c>
@@ -3310,14 +3482,12 @@
       <c r="AW14" s="43"/>
       <c r="AX14" s="43"/>
       <c r="AY14" s="43"/>
-      <c r="AZ14" s="43"/>
-      <c r="BA14" s="43"/>
-    </row>
-    <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="47"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
+      <c r="D15" s="126"/>
       <c r="E15" s="44" t="s">
         <v>15</v>
       </c>
@@ -3365,81 +3535,79 @@
       <c r="AW15" s="43"/>
       <c r="AX15" s="43"/>
       <c r="AY15" s="43"/>
-      <c r="AZ15" s="43"/>
-      <c r="BA15" s="43"/>
-    </row>
-    <row r="16" spans="1:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:57" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A16" s="47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B16" s="53">
         <f>SUM(B3:B15)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C16" s="53">
         <f>SUM(C3:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="105"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="99"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="99"/>
-      <c r="S16" s="99"/>
-      <c r="T16" s="99"/>
-      <c r="U16" s="99"/>
-      <c r="V16" s="99"/>
-      <c r="W16" s="99"/>
-      <c r="X16" s="99"/>
-      <c r="Y16" s="99"/>
-      <c r="Z16" s="99"/>
-      <c r="AA16" s="99"/>
-      <c r="AB16" s="99"/>
-      <c r="AC16" s="99"/>
-      <c r="AD16" s="99"/>
-      <c r="AE16" s="99"/>
-      <c r="AF16" s="99"/>
-      <c r="AG16" s="99"/>
-      <c r="AH16" s="99"/>
-      <c r="AI16" s="99"/>
-      <c r="AJ16" s="99"/>
-      <c r="AK16" s="99"/>
-      <c r="AL16" s="99"/>
-      <c r="AM16" s="99"/>
-      <c r="AN16" s="99"/>
-      <c r="AO16" s="99"/>
-      <c r="AP16" s="99"/>
-      <c r="AQ16" s="99"/>
-      <c r="AR16" s="99"/>
-      <c r="AS16" s="99"/>
-      <c r="AT16" s="99"/>
-      <c r="AU16" s="99"/>
-      <c r="AV16" s="99"/>
-      <c r="AW16" s="99"/>
-      <c r="AX16" s="99"/>
-      <c r="AY16" s="99"/>
-      <c r="AZ16" s="99"/>
-      <c r="BA16" s="99"/>
-      <c r="BB16" s="99"/>
-      <c r="BC16" s="99"/>
-    </row>
-    <row r="17" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="104" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
+        <v>30</v>
+      </c>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="100"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="100"/>
+      <c r="N16" s="100"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="100"/>
+      <c r="Q16" s="100"/>
+      <c r="R16" s="100"/>
+      <c r="S16" s="100"/>
+      <c r="T16" s="100"/>
+      <c r="U16" s="100"/>
+      <c r="V16" s="100"/>
+      <c r="W16" s="100"/>
+      <c r="X16" s="100"/>
+      <c r="Y16" s="100"/>
+      <c r="Z16" s="100"/>
+      <c r="AA16" s="100"/>
+      <c r="AB16" s="100"/>
+      <c r="AC16" s="100"/>
+      <c r="AD16" s="100"/>
+      <c r="AE16" s="100"/>
+      <c r="AF16" s="100"/>
+      <c r="AG16" s="100"/>
+      <c r="AH16" s="100"/>
+      <c r="AI16" s="100"/>
+      <c r="AJ16" s="100"/>
+      <c r="AK16" s="100"/>
+      <c r="AL16" s="100"/>
+      <c r="AM16" s="100"/>
+      <c r="AN16" s="100"/>
+      <c r="AO16" s="100"/>
+      <c r="AP16" s="100"/>
+      <c r="AQ16" s="100"/>
+      <c r="AR16" s="100"/>
+      <c r="AS16" s="100"/>
+      <c r="AT16" s="100"/>
+      <c r="AU16" s="100"/>
+      <c r="AV16" s="100"/>
+      <c r="AW16" s="100"/>
+      <c r="AX16" s="100"/>
+      <c r="AY16" s="100"/>
+      <c r="AZ16" s="100"/>
+      <c r="BA16" s="100"/>
+      <c r="BB16" s="100"/>
+      <c r="BC16" s="100"/>
+    </row>
+    <row r="17" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
       <c r="E17" s="45"/>
       <c r="F17" s="45">
         <v>1</v>
@@ -3641,9 +3809,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A18" s="46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B18" s="49">
         <v>1</v>
@@ -3711,9 +3879,9 @@
       <c r="BB18" s="43"/>
       <c r="BC18" s="43"/>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B19" s="51">
         <v>2</v>
@@ -3787,9 +3955,9 @@
       <c r="BB19" s="43"/>
       <c r="BC19" s="43"/>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A20" s="47" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B20" s="51">
         <v>4</v>
@@ -3866,7 +4034,7 @@
       <c r="BB20" s="43"/>
       <c r="BC20" s="43"/>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A21" s="47"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
@@ -3925,7 +4093,7 @@
       <c r="BB21" s="43"/>
       <c r="BC21" s="43"/>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A22" s="47"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
@@ -3984,7 +4152,7 @@
       <c r="BB22" s="43"/>
       <c r="BC22" s="43"/>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A23" s="47"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
@@ -4043,7 +4211,7 @@
       <c r="BB23" s="43"/>
       <c r="BC23" s="43"/>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A24" s="47"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
@@ -4102,7 +4270,7 @@
       <c r="BB24" s="43"/>
       <c r="BC24" s="43"/>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A25" s="47"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
@@ -4161,7 +4329,7 @@
       <c r="BB25" s="43"/>
       <c r="BC25" s="43"/>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A26" s="47"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
@@ -4220,7 +4388,7 @@
       <c r="BB26" s="43"/>
       <c r="BC26" s="43"/>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A27" s="47"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
@@ -4279,7 +4447,7 @@
       <c r="BB27" s="43"/>
       <c r="BC27" s="43"/>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A28" s="47"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
@@ -4338,7 +4506,7 @@
       <c r="BB28" s="43"/>
       <c r="BC28" s="43"/>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A29" s="47"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
@@ -4397,7 +4565,7 @@
       <c r="BB29" s="43"/>
       <c r="BC29" s="43"/>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A30" s="47"/>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
@@ -4456,7 +4624,7 @@
       <c r="BB30" s="43"/>
       <c r="BC30" s="43"/>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A31" s="47"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
@@ -4515,7 +4683,7 @@
       <c r="BB31" s="43"/>
       <c r="BC31" s="43"/>
     </row>
-    <row r="32" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="47"/>
       <c r="B32" s="51"/>
       <c r="C32" s="51"/>
@@ -4574,9 +4742,9 @@
       <c r="BB32" s="43"/>
       <c r="BC32" s="43"/>
     </row>
-    <row r="33" spans="1:57" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:57" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A33" s="47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B33" s="53">
         <f>SUM(B18:B32)</f>
@@ -4586,66 +4754,66 @@
         <f>SUM(C18:C32)</f>
         <v>6</v>
       </c>
-      <c r="D33" s="102"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="101"/>
-      <c r="H33" s="101"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="101"/>
-      <c r="L33" s="101"/>
-      <c r="M33" s="101"/>
-      <c r="N33" s="101"/>
-      <c r="O33" s="101"/>
-      <c r="P33" s="101"/>
-      <c r="Q33" s="101"/>
-      <c r="R33" s="101"/>
-      <c r="S33" s="101"/>
-      <c r="T33" s="101"/>
-      <c r="U33" s="101"/>
-      <c r="V33" s="101"/>
-      <c r="W33" s="101"/>
-      <c r="X33" s="101"/>
-      <c r="Y33" s="101"/>
-      <c r="Z33" s="101"/>
-      <c r="AA33" s="101"/>
-      <c r="AB33" s="101"/>
-      <c r="AC33" s="101"/>
-      <c r="AD33" s="101"/>
-      <c r="AE33" s="101"/>
-      <c r="AF33" s="101"/>
-      <c r="AG33" s="101"/>
-      <c r="AH33" s="101"/>
-      <c r="AI33" s="101"/>
-      <c r="AJ33" s="101"/>
-      <c r="AK33" s="101"/>
-      <c r="AL33" s="101"/>
-      <c r="AM33" s="101"/>
-      <c r="AN33" s="101"/>
-      <c r="AO33" s="101"/>
-      <c r="AP33" s="101"/>
-      <c r="AQ33" s="101"/>
-      <c r="AR33" s="101"/>
-      <c r="AS33" s="101"/>
-      <c r="AT33" s="101"/>
-      <c r="AU33" s="101"/>
-      <c r="AV33" s="101"/>
-      <c r="AW33" s="101"/>
-      <c r="AX33" s="101"/>
-      <c r="AY33" s="101"/>
-      <c r="AZ33" s="101"/>
-      <c r="BA33" s="101"/>
-      <c r="BB33" s="101"/>
-      <c r="BC33" s="101"/>
-    </row>
-    <row r="34" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="104" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="104"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="102"/>
+      <c r="K33" s="102"/>
+      <c r="L33" s="102"/>
+      <c r="M33" s="102"/>
+      <c r="N33" s="102"/>
+      <c r="O33" s="102"/>
+      <c r="P33" s="102"/>
+      <c r="Q33" s="102"/>
+      <c r="R33" s="102"/>
+      <c r="S33" s="102"/>
+      <c r="T33" s="102"/>
+      <c r="U33" s="102"/>
+      <c r="V33" s="102"/>
+      <c r="W33" s="102"/>
+      <c r="X33" s="102"/>
+      <c r="Y33" s="102"/>
+      <c r="Z33" s="102"/>
+      <c r="AA33" s="102"/>
+      <c r="AB33" s="102"/>
+      <c r="AC33" s="102"/>
+      <c r="AD33" s="102"/>
+      <c r="AE33" s="102"/>
+      <c r="AF33" s="102"/>
+      <c r="AG33" s="102"/>
+      <c r="AH33" s="102"/>
+      <c r="AI33" s="102"/>
+      <c r="AJ33" s="102"/>
+      <c r="AK33" s="102"/>
+      <c r="AL33" s="102"/>
+      <c r="AM33" s="102"/>
+      <c r="AN33" s="102"/>
+      <c r="AO33" s="102"/>
+      <c r="AP33" s="102"/>
+      <c r="AQ33" s="102"/>
+      <c r="AR33" s="102"/>
+      <c r="AS33" s="102"/>
+      <c r="AT33" s="102"/>
+      <c r="AU33" s="102"/>
+      <c r="AV33" s="102"/>
+      <c r="AW33" s="102"/>
+      <c r="AX33" s="102"/>
+      <c r="AY33" s="102"/>
+      <c r="AZ33" s="102"/>
+      <c r="BA33" s="102"/>
+      <c r="BB33" s="102"/>
+      <c r="BC33" s="102"/>
+    </row>
+    <row r="34" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="94"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
       <c r="E34" s="45"/>
       <c r="F34" s="45">
         <v>1</v>
@@ -4847,9 +5015,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A35" s="46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="49"/>
@@ -4910,7 +5078,7 @@
       <c r="BD35" s="43"/>
       <c r="BE35" s="43"/>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A36" s="47"/>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
@@ -4971,7 +5139,7 @@
       <c r="BD36" s="43"/>
       <c r="BE36" s="43"/>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A37" s="47"/>
       <c r="B37" s="51"/>
       <c r="C37" s="51"/>
@@ -5032,7 +5200,7 @@
       <c r="BD37" s="43"/>
       <c r="BE37" s="43"/>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A38" s="47"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
@@ -5093,7 +5261,7 @@
       <c r="BD38" s="43"/>
       <c r="BE38" s="43"/>
     </row>
-    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A39" s="47"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
@@ -5154,7 +5322,7 @@
       <c r="BD39" s="43"/>
       <c r="BE39" s="43"/>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A40" s="47"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
@@ -5215,7 +5383,7 @@
       <c r="BD40" s="43"/>
       <c r="BE40" s="43"/>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A41" s="47"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -5276,7 +5444,7 @@
       <c r="BD41" s="43"/>
       <c r="BE41" s="43"/>
     </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A42" s="47"/>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -5337,7 +5505,7 @@
       <c r="BD42" s="43"/>
       <c r="BE42" s="43"/>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A43" s="47"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
@@ -5398,7 +5566,7 @@
       <c r="BD43" s="43"/>
       <c r="BE43" s="43"/>
     </row>
-    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A44" s="47"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -5459,7 +5627,7 @@
       <c r="BD44" s="43"/>
       <c r="BE44" s="43"/>
     </row>
-    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:57" x14ac:dyDescent="0.4">
       <c r="A45" s="47"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
@@ -5520,7 +5688,7 @@
       <c r="BD45" s="43"/>
       <c r="BE45" s="43"/>
     </row>
-    <row r="46" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="47"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -5581,9 +5749,9 @@
       <c r="BD46" s="43"/>
       <c r="BE46" s="43"/>
     </row>
-    <row r="47" spans="1:57" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:57" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A47" s="47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B47" s="53">
         <f>SUM(B35:B46)</f>
@@ -5593,68 +5761,68 @@
         <f>SUM(C35:C46)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="102"/>
-      <c r="E47" s="102"/>
-      <c r="F47" s="100"/>
-      <c r="G47" s="101"/>
-      <c r="H47" s="101"/>
-      <c r="I47" s="101"/>
-      <c r="J47" s="101"/>
-      <c r="K47" s="101"/>
-      <c r="L47" s="101"/>
-      <c r="M47" s="101"/>
-      <c r="N47" s="101"/>
-      <c r="O47" s="101"/>
-      <c r="P47" s="101"/>
-      <c r="Q47" s="101"/>
-      <c r="R47" s="101"/>
-      <c r="S47" s="101"/>
-      <c r="T47" s="101"/>
-      <c r="U47" s="101"/>
-      <c r="V47" s="101"/>
-      <c r="W47" s="101"/>
-      <c r="X47" s="101"/>
-      <c r="Y47" s="101"/>
-      <c r="Z47" s="101"/>
-      <c r="AA47" s="101"/>
-      <c r="AB47" s="101"/>
-      <c r="AC47" s="101"/>
-      <c r="AD47" s="101"/>
-      <c r="AE47" s="101"/>
-      <c r="AF47" s="101"/>
-      <c r="AG47" s="101"/>
-      <c r="AH47" s="101"/>
-      <c r="AI47" s="101"/>
-      <c r="AJ47" s="101"/>
-      <c r="AK47" s="101"/>
-      <c r="AL47" s="101"/>
-      <c r="AM47" s="101"/>
-      <c r="AN47" s="101"/>
-      <c r="AO47" s="101"/>
-      <c r="AP47" s="101"/>
-      <c r="AQ47" s="101"/>
-      <c r="AR47" s="101"/>
-      <c r="AS47" s="101"/>
-      <c r="AT47" s="101"/>
-      <c r="AU47" s="101"/>
-      <c r="AV47" s="101"/>
-      <c r="AW47" s="101"/>
-      <c r="AX47" s="101"/>
-      <c r="AY47" s="101"/>
-      <c r="AZ47" s="101"/>
-      <c r="BA47" s="101"/>
-      <c r="BB47" s="101"/>
-      <c r="BC47" s="101"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="101"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="102"/>
+      <c r="I47" s="102"/>
+      <c r="J47" s="102"/>
+      <c r="K47" s="102"/>
+      <c r="L47" s="102"/>
+      <c r="M47" s="102"/>
+      <c r="N47" s="102"/>
+      <c r="O47" s="102"/>
+      <c r="P47" s="102"/>
+      <c r="Q47" s="102"/>
+      <c r="R47" s="102"/>
+      <c r="S47" s="102"/>
+      <c r="T47" s="102"/>
+      <c r="U47" s="102"/>
+      <c r="V47" s="102"/>
+      <c r="W47" s="102"/>
+      <c r="X47" s="102"/>
+      <c r="Y47" s="102"/>
+      <c r="Z47" s="102"/>
+      <c r="AA47" s="102"/>
+      <c r="AB47" s="102"/>
+      <c r="AC47" s="102"/>
+      <c r="AD47" s="102"/>
+      <c r="AE47" s="102"/>
+      <c r="AF47" s="102"/>
+      <c r="AG47" s="102"/>
+      <c r="AH47" s="102"/>
+      <c r="AI47" s="102"/>
+      <c r="AJ47" s="102"/>
+      <c r="AK47" s="102"/>
+      <c r="AL47" s="102"/>
+      <c r="AM47" s="102"/>
+      <c r="AN47" s="102"/>
+      <c r="AO47" s="102"/>
+      <c r="AP47" s="102"/>
+      <c r="AQ47" s="102"/>
+      <c r="AR47" s="102"/>
+      <c r="AS47" s="102"/>
+      <c r="AT47" s="102"/>
+      <c r="AU47" s="102"/>
+      <c r="AV47" s="102"/>
+      <c r="AW47" s="102"/>
+      <c r="AX47" s="102"/>
+      <c r="AY47" s="102"/>
+      <c r="AZ47" s="102"/>
+      <c r="BA47" s="102"/>
+      <c r="BB47" s="102"/>
+      <c r="BC47" s="102"/>
       <c r="BD47" s="43"/>
       <c r="BE47" s="43"/>
     </row>
-    <row r="48" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="104" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="104"/>
-      <c r="C48" s="104"/>
-      <c r="D48" s="104"/>
+    <row r="48" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="94" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="94"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="94"/>
       <c r="E48" s="45"/>
       <c r="F48" s="45">
         <v>1</v>
@@ -5856,9 +6024,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A49" s="46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B49" s="49"/>
       <c r="C49" s="49"/>
@@ -5917,7 +6085,7 @@
       <c r="BB49" s="43"/>
       <c r="BC49" s="43"/>
     </row>
-    <row r="50" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A50" s="47"/>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
@@ -5976,7 +6144,7 @@
       <c r="BB50" s="43"/>
       <c r="BC50" s="43"/>
     </row>
-    <row r="51" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A51" s="47"/>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -6035,7 +6203,7 @@
       <c r="BB51" s="43"/>
       <c r="BC51" s="43"/>
     </row>
-    <row r="52" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A52" s="47"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
@@ -6094,7 +6262,7 @@
       <c r="BB52" s="43"/>
       <c r="BC52" s="43"/>
     </row>
-    <row r="53" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A53" s="47"/>
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
@@ -6153,7 +6321,7 @@
       <c r="BB53" s="43"/>
       <c r="BC53" s="43"/>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A54" s="47"/>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
@@ -6212,7 +6380,7 @@
       <c r="BB54" s="43"/>
       <c r="BC54" s="43"/>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A55" s="47"/>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
@@ -6271,7 +6439,7 @@
       <c r="BB55" s="43"/>
       <c r="BC55" s="43"/>
     </row>
-    <row r="56" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A56" s="47"/>
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
@@ -6330,7 +6498,7 @@
       <c r="BB56" s="43"/>
       <c r="BC56" s="43"/>
     </row>
-    <row r="57" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A57" s="47"/>
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
@@ -6389,7 +6557,7 @@
       <c r="BB57" s="43"/>
       <c r="BC57" s="43"/>
     </row>
-    <row r="58" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A58" s="47"/>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
@@ -6448,7 +6616,7 @@
       <c r="BB58" s="43"/>
       <c r="BC58" s="43"/>
     </row>
-    <row r="59" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A59" s="47"/>
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
@@ -6507,7 +6675,7 @@
       <c r="BB59" s="43"/>
       <c r="BC59" s="43"/>
     </row>
-    <row r="60" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="47"/>
       <c r="B60" s="51"/>
       <c r="C60" s="51"/>
@@ -6566,9 +6734,9 @@
       <c r="BB60" s="43"/>
       <c r="BC60" s="43"/>
     </row>
-    <row r="61" spans="1:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A61" s="47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B61" s="53">
         <f>SUM(B49:B60)</f>
@@ -6578,66 +6746,66 @@
         <f>SUM(C49:C60)</f>
         <v>0</v>
       </c>
-      <c r="D61" s="102"/>
-      <c r="E61" s="102"/>
-      <c r="F61" s="100"/>
-      <c r="G61" s="101"/>
-      <c r="H61" s="101"/>
-      <c r="I61" s="101"/>
-      <c r="J61" s="101"/>
-      <c r="K61" s="101"/>
-      <c r="L61" s="101"/>
-      <c r="M61" s="101"/>
-      <c r="N61" s="101"/>
-      <c r="O61" s="101"/>
-      <c r="P61" s="101"/>
-      <c r="Q61" s="101"/>
-      <c r="R61" s="101"/>
-      <c r="S61" s="101"/>
-      <c r="T61" s="101"/>
-      <c r="U61" s="101"/>
-      <c r="V61" s="101"/>
-      <c r="W61" s="101"/>
-      <c r="X61" s="101"/>
-      <c r="Y61" s="101"/>
-      <c r="Z61" s="101"/>
-      <c r="AA61" s="101"/>
-      <c r="AB61" s="101"/>
-      <c r="AC61" s="101"/>
-      <c r="AD61" s="101"/>
-      <c r="AE61" s="101"/>
-      <c r="AF61" s="101"/>
-      <c r="AG61" s="101"/>
-      <c r="AH61" s="101"/>
-      <c r="AI61" s="101"/>
-      <c r="AJ61" s="101"/>
-      <c r="AK61" s="101"/>
-      <c r="AL61" s="101"/>
-      <c r="AM61" s="101"/>
-      <c r="AN61" s="101"/>
-      <c r="AO61" s="101"/>
-      <c r="AP61" s="101"/>
-      <c r="AQ61" s="101"/>
-      <c r="AR61" s="101"/>
-      <c r="AS61" s="101"/>
-      <c r="AT61" s="101"/>
-      <c r="AU61" s="101"/>
-      <c r="AV61" s="101"/>
-      <c r="AW61" s="101"/>
-      <c r="AX61" s="101"/>
-      <c r="AY61" s="101"/>
-      <c r="AZ61" s="101"/>
-      <c r="BA61" s="101"/>
-      <c r="BB61" s="101"/>
-      <c r="BC61" s="101"/>
-    </row>
-    <row r="62" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="104" t="s">
-        <v>49</v>
-      </c>
-      <c r="B62" s="104"/>
-      <c r="C62" s="104"/>
-      <c r="D62" s="104"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="96"/>
+      <c r="F61" s="101"/>
+      <c r="G61" s="102"/>
+      <c r="H61" s="102"/>
+      <c r="I61" s="102"/>
+      <c r="J61" s="102"/>
+      <c r="K61" s="102"/>
+      <c r="L61" s="102"/>
+      <c r="M61" s="102"/>
+      <c r="N61" s="102"/>
+      <c r="O61" s="102"/>
+      <c r="P61" s="102"/>
+      <c r="Q61" s="102"/>
+      <c r="R61" s="102"/>
+      <c r="S61" s="102"/>
+      <c r="T61" s="102"/>
+      <c r="U61" s="102"/>
+      <c r="V61" s="102"/>
+      <c r="W61" s="102"/>
+      <c r="X61" s="102"/>
+      <c r="Y61" s="102"/>
+      <c r="Z61" s="102"/>
+      <c r="AA61" s="102"/>
+      <c r="AB61" s="102"/>
+      <c r="AC61" s="102"/>
+      <c r="AD61" s="102"/>
+      <c r="AE61" s="102"/>
+      <c r="AF61" s="102"/>
+      <c r="AG61" s="102"/>
+      <c r="AH61" s="102"/>
+      <c r="AI61" s="102"/>
+      <c r="AJ61" s="102"/>
+      <c r="AK61" s="102"/>
+      <c r="AL61" s="102"/>
+      <c r="AM61" s="102"/>
+      <c r="AN61" s="102"/>
+      <c r="AO61" s="102"/>
+      <c r="AP61" s="102"/>
+      <c r="AQ61" s="102"/>
+      <c r="AR61" s="102"/>
+      <c r="AS61" s="102"/>
+      <c r="AT61" s="102"/>
+      <c r="AU61" s="102"/>
+      <c r="AV61" s="102"/>
+      <c r="AW61" s="102"/>
+      <c r="AX61" s="102"/>
+      <c r="AY61" s="102"/>
+      <c r="AZ61" s="102"/>
+      <c r="BA61" s="102"/>
+      <c r="BB61" s="102"/>
+      <c r="BC61" s="102"/>
+    </row>
+    <row r="62" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="94"/>
+      <c r="C62" s="94"/>
+      <c r="D62" s="94"/>
       <c r="E62" s="45"/>
       <c r="F62" s="45">
         <v>1</v>
@@ -6839,9 +7007,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A63" s="46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B63" s="49"/>
       <c r="C63" s="49"/>
@@ -6900,7 +7068,7 @@
       <c r="BB63" s="43"/>
       <c r="BC63" s="43"/>
     </row>
-    <row r="64" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A64" s="47"/>
       <c r="B64" s="51"/>
       <c r="C64" s="51"/>
@@ -6959,7 +7127,7 @@
       <c r="BB64" s="43"/>
       <c r="BC64" s="43"/>
     </row>
-    <row r="65" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A65" s="48"/>
       <c r="B65" s="51"/>
       <c r="C65" s="51"/>
@@ -7018,7 +7186,7 @@
       <c r="BB65" s="43"/>
       <c r="BC65" s="43"/>
     </row>
-    <row r="66" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A66" s="47"/>
       <c r="B66" s="51"/>
       <c r="C66" s="51"/>
@@ -7077,7 +7245,7 @@
       <c r="BB66" s="43"/>
       <c r="BC66" s="43"/>
     </row>
-    <row r="67" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A67" s="47"/>
       <c r="B67" s="51"/>
       <c r="C67" s="51"/>
@@ -7136,7 +7304,7 @@
       <c r="BB67" s="43"/>
       <c r="BC67" s="43"/>
     </row>
-    <row r="68" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A68" s="47"/>
       <c r="B68" s="51"/>
       <c r="C68" s="51"/>
@@ -7195,7 +7363,7 @@
       <c r="BB68" s="43"/>
       <c r="BC68" s="43"/>
     </row>
-    <row r="69" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A69" s="47"/>
       <c r="B69" s="51"/>
       <c r="C69" s="51"/>
@@ -7254,7 +7422,7 @@
       <c r="BB69" s="43"/>
       <c r="BC69" s="43"/>
     </row>
-    <row r="70" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A70" s="47"/>
       <c r="B70" s="51"/>
       <c r="C70" s="51"/>
@@ -7313,7 +7481,7 @@
       <c r="BB70" s="43"/>
       <c r="BC70" s="43"/>
     </row>
-    <row r="71" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A71" s="47"/>
       <c r="B71" s="51"/>
       <c r="C71" s="51"/>
@@ -7372,7 +7540,7 @@
       <c r="BB71" s="43"/>
       <c r="BC71" s="43"/>
     </row>
-    <row r="72" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A72" s="47"/>
       <c r="B72" s="51"/>
       <c r="C72" s="51"/>
@@ -7431,7 +7599,7 @@
       <c r="BB72" s="43"/>
       <c r="BC72" s="43"/>
     </row>
-    <row r="73" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A73" s="47"/>
       <c r="B73" s="51"/>
       <c r="C73" s="51"/>
@@ -7490,7 +7658,7 @@
       <c r="BB73" s="43"/>
       <c r="BC73" s="43"/>
     </row>
-    <row r="74" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A74" s="47"/>
       <c r="B74" s="51"/>
       <c r="C74" s="51"/>
@@ -7549,7 +7717,7 @@
       <c r="BB74" s="43"/>
       <c r="BC74" s="43"/>
     </row>
-    <row r="75" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:55" x14ac:dyDescent="0.4">
       <c r="A75" s="47"/>
       <c r="B75" s="51"/>
       <c r="C75" s="51"/>
@@ -7608,7 +7776,7 @@
       <c r="BB75" s="43"/>
       <c r="BC75" s="43"/>
     </row>
-    <row r="76" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A76" s="47"/>
       <c r="B76" s="51"/>
       <c r="C76" s="51"/>
@@ -7667,9 +7835,9 @@
       <c r="BB76" s="43"/>
       <c r="BC76" s="43"/>
     </row>
-    <row r="77" spans="1:55" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:55" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A77" s="47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B77" s="53">
         <f>SUM(B63:B76)</f>
@@ -7679,200 +7847,194 @@
         <f>SUM(C63:C75)</f>
         <v>0</v>
       </c>
-      <c r="D77" s="102"/>
-      <c r="E77" s="102"/>
-      <c r="F77" s="100"/>
-      <c r="G77" s="101"/>
-      <c r="H77" s="101"/>
-      <c r="I77" s="101"/>
-      <c r="J77" s="101"/>
-      <c r="K77" s="101"/>
-      <c r="L77" s="101"/>
-      <c r="M77" s="101"/>
-      <c r="N77" s="101"/>
-      <c r="O77" s="101"/>
-      <c r="P77" s="101"/>
-      <c r="Q77" s="101"/>
-      <c r="R77" s="101"/>
-      <c r="S77" s="101"/>
-      <c r="T77" s="101"/>
-      <c r="U77" s="101"/>
-      <c r="V77" s="101"/>
-      <c r="W77" s="101"/>
-      <c r="X77" s="101"/>
-      <c r="Y77" s="101"/>
-      <c r="Z77" s="101"/>
-      <c r="AA77" s="101"/>
-      <c r="AB77" s="101"/>
-      <c r="AC77" s="101"/>
-      <c r="AD77" s="101"/>
-      <c r="AE77" s="101"/>
-      <c r="AF77" s="101"/>
-      <c r="AG77" s="101"/>
-      <c r="AH77" s="101"/>
-      <c r="AI77" s="101"/>
-      <c r="AJ77" s="101"/>
-      <c r="AK77" s="101"/>
-      <c r="AL77" s="101"/>
-      <c r="AM77" s="101"/>
-      <c r="AN77" s="101"/>
-      <c r="AO77" s="101"/>
-      <c r="AP77" s="101"/>
-      <c r="AQ77" s="101"/>
-      <c r="AR77" s="101"/>
-      <c r="AS77" s="101"/>
-      <c r="AT77" s="101"/>
-      <c r="AU77" s="101"/>
-      <c r="AV77" s="101"/>
-      <c r="AW77" s="101"/>
-      <c r="AX77" s="101"/>
-      <c r="AY77" s="101"/>
-      <c r="AZ77" s="101"/>
-      <c r="BA77" s="101"/>
-      <c r="BB77" s="101"/>
-      <c r="BC77" s="101"/>
-    </row>
-    <row r="78" spans="1:55" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="96"/>
+      <c r="E77" s="96"/>
+      <c r="F77" s="101"/>
+      <c r="G77" s="102"/>
+      <c r="H77" s="102"/>
+      <c r="I77" s="102"/>
+      <c r="J77" s="102"/>
+      <c r="K77" s="102"/>
+      <c r="L77" s="102"/>
+      <c r="M77" s="102"/>
+      <c r="N77" s="102"/>
+      <c r="O77" s="102"/>
+      <c r="P77" s="102"/>
+      <c r="Q77" s="102"/>
+      <c r="R77" s="102"/>
+      <c r="S77" s="102"/>
+      <c r="T77" s="102"/>
+      <c r="U77" s="102"/>
+      <c r="V77" s="102"/>
+      <c r="W77" s="102"/>
+      <c r="X77" s="102"/>
+      <c r="Y77" s="102"/>
+      <c r="Z77" s="102"/>
+      <c r="AA77" s="102"/>
+      <c r="AB77" s="102"/>
+      <c r="AC77" s="102"/>
+      <c r="AD77" s="102"/>
+      <c r="AE77" s="102"/>
+      <c r="AF77" s="102"/>
+      <c r="AG77" s="102"/>
+      <c r="AH77" s="102"/>
+      <c r="AI77" s="102"/>
+      <c r="AJ77" s="102"/>
+      <c r="AK77" s="102"/>
+      <c r="AL77" s="102"/>
+      <c r="AM77" s="102"/>
+      <c r="AN77" s="102"/>
+      <c r="AO77" s="102"/>
+      <c r="AP77" s="102"/>
+      <c r="AQ77" s="102"/>
+      <c r="AR77" s="102"/>
+      <c r="AS77" s="102"/>
+      <c r="AT77" s="102"/>
+      <c r="AU77" s="102"/>
+      <c r="AV77" s="102"/>
+      <c r="AW77" s="102"/>
+      <c r="AX77" s="102"/>
+      <c r="AY77" s="102"/>
+      <c r="AZ77" s="102"/>
+      <c r="BA77" s="102"/>
+      <c r="BB77" s="102"/>
+      <c r="BC77" s="102"/>
+    </row>
+    <row r="78" spans="1:55" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A78" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B78" s="56" t="e">
-        <f>SUM(B61,B77,#REF!,B16, B47,#REF!, B33)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C78" s="56" t="e">
-        <f>SUM(C16,C33,#REF!,C47,#REF!,C61,C77)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D78" s="96"/>
-      <c r="E78" s="96"/>
-      <c r="F78" s="96"/>
-      <c r="G78" s="96"/>
-      <c r="H78" s="96"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="96"/>
-      <c r="K78" s="96"/>
-      <c r="L78" s="96"/>
-      <c r="M78" s="96"/>
-      <c r="N78" s="96"/>
-      <c r="O78" s="96"/>
-      <c r="P78" s="96"/>
-      <c r="Q78" s="96"/>
-      <c r="R78" s="96"/>
-      <c r="S78" s="96"/>
-      <c r="T78" s="96"/>
-      <c r="U78" s="96"/>
-      <c r="V78" s="96"/>
-      <c r="W78" s="96"/>
-      <c r="X78" s="96"/>
-      <c r="Y78" s="96"/>
-      <c r="Z78" s="96"/>
-      <c r="AA78" s="96"/>
-      <c r="AB78" s="96"/>
-      <c r="AC78" s="96"/>
-      <c r="AD78" s="96"/>
-      <c r="AE78" s="96"/>
-      <c r="AF78" s="96"/>
-      <c r="AG78" s="96"/>
-      <c r="AH78" s="96"/>
-      <c r="AI78" s="96"/>
-      <c r="AJ78" s="96"/>
-      <c r="AK78" s="96"/>
-      <c r="AL78" s="96"/>
-      <c r="AM78" s="96"/>
-      <c r="AN78" s="96"/>
-      <c r="AO78" s="96"/>
-      <c r="AP78" s="96"/>
-      <c r="AQ78" s="96"/>
-      <c r="AR78" s="96"/>
-      <c r="AS78" s="96"/>
-      <c r="AT78" s="96"/>
-      <c r="AU78" s="96"/>
-      <c r="AV78" s="96"/>
-      <c r="AW78" s="96"/>
-      <c r="AX78" s="96"/>
-      <c r="AY78" s="96"/>
-      <c r="AZ78" s="96"/>
-      <c r="BA78" s="96"/>
-      <c r="BB78" s="96"/>
-      <c r="BC78" s="96"/>
-    </row>
-    <row r="79" spans="1:55" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="56">
+        <f>SUM(B61,B77,B16, B47, B33)</f>
+        <v>60</v>
+      </c>
+      <c r="C78" s="56">
+        <f>SUM(C16,C33,C47,C61,C77)</f>
+        <v>36</v>
+      </c>
+      <c r="D78" s="97"/>
+      <c r="E78" s="97"/>
+      <c r="F78" s="97"/>
+      <c r="G78" s="97"/>
+      <c r="H78" s="97"/>
+      <c r="I78" s="97"/>
+      <c r="J78" s="97"/>
+      <c r="K78" s="97"/>
+      <c r="L78" s="97"/>
+      <c r="M78" s="97"/>
+      <c r="N78" s="97"/>
+      <c r="O78" s="97"/>
+      <c r="P78" s="97"/>
+      <c r="Q78" s="97"/>
+      <c r="R78" s="97"/>
+      <c r="S78" s="97"/>
+      <c r="T78" s="97"/>
+      <c r="U78" s="97"/>
+      <c r="V78" s="97"/>
+      <c r="W78" s="97"/>
+      <c r="X78" s="97"/>
+      <c r="Y78" s="97"/>
+      <c r="Z78" s="97"/>
+      <c r="AA78" s="97"/>
+      <c r="AB78" s="97"/>
+      <c r="AC78" s="97"/>
+      <c r="AD78" s="97"/>
+      <c r="AE78" s="97"/>
+      <c r="AF78" s="97"/>
+      <c r="AG78" s="97"/>
+      <c r="AH78" s="97"/>
+      <c r="AI78" s="97"/>
+      <c r="AJ78" s="97"/>
+      <c r="AK78" s="97"/>
+      <c r="AL78" s="97"/>
+      <c r="AM78" s="97"/>
+      <c r="AN78" s="97"/>
+      <c r="AO78" s="97"/>
+      <c r="AP78" s="97"/>
+      <c r="AQ78" s="97"/>
+      <c r="AR78" s="97"/>
+      <c r="AS78" s="97"/>
+      <c r="AT78" s="97"/>
+      <c r="AU78" s="97"/>
+      <c r="AV78" s="97"/>
+      <c r="AW78" s="97"/>
+      <c r="AX78" s="97"/>
+      <c r="AY78" s="97"/>
+      <c r="AZ78" s="97"/>
+      <c r="BA78" s="97"/>
+      <c r="BB78" s="97"/>
+      <c r="BC78" s="97"/>
+    </row>
+    <row r="79" spans="1:55" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A79" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="58" t="e">
+      <c r="B79" s="58">
         <f>B78*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C79" s="58" t="e">
+        <v>6000</v>
+      </c>
+      <c r="C79" s="58">
         <f>C78*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D79" s="97"/>
-      <c r="E79" s="97"/>
-      <c r="F79" s="97"/>
-      <c r="G79" s="97"/>
-      <c r="H79" s="97"/>
-      <c r="I79" s="97"/>
-      <c r="J79" s="97"/>
-      <c r="K79" s="97"/>
-      <c r="L79" s="97"/>
-      <c r="M79" s="97"/>
-      <c r="N79" s="97"/>
-      <c r="O79" s="97"/>
-      <c r="P79" s="97"/>
-      <c r="Q79" s="97"/>
-      <c r="R79" s="97"/>
-      <c r="S79" s="97"/>
-      <c r="T79" s="97"/>
-      <c r="U79" s="97"/>
-      <c r="V79" s="97"/>
-      <c r="W79" s="97"/>
-      <c r="X79" s="97"/>
-      <c r="Y79" s="97"/>
-      <c r="Z79" s="97"/>
-      <c r="AA79" s="97"/>
-      <c r="AB79" s="97"/>
-      <c r="AC79" s="97"/>
-      <c r="AD79" s="97"/>
-      <c r="AE79" s="97"/>
-      <c r="AF79" s="97"/>
-      <c r="AG79" s="97"/>
-      <c r="AH79" s="97"/>
-      <c r="AI79" s="97"/>
-      <c r="AJ79" s="97"/>
-      <c r="AK79" s="97"/>
-      <c r="AL79" s="97"/>
-      <c r="AM79" s="97"/>
-      <c r="AN79" s="97"/>
-      <c r="AO79" s="97"/>
-      <c r="AP79" s="97"/>
-      <c r="AQ79" s="97"/>
-      <c r="AR79" s="97"/>
-      <c r="AS79" s="97"/>
-      <c r="AT79" s="97"/>
-      <c r="AU79" s="97"/>
-      <c r="AV79" s="97"/>
-      <c r="AW79" s="97"/>
-      <c r="AX79" s="97"/>
-      <c r="AY79" s="97"/>
-      <c r="AZ79" s="97"/>
-      <c r="BA79" s="97"/>
-      <c r="BB79" s="97"/>
-      <c r="BC79" s="97"/>
-    </row>
-    <row r="94" spans="55:55" x14ac:dyDescent="0.25">
+        <v>3600</v>
+      </c>
+      <c r="D79" s="98"/>
+      <c r="E79" s="98"/>
+      <c r="F79" s="98"/>
+      <c r="G79" s="98"/>
+      <c r="H79" s="98"/>
+      <c r="I79" s="98"/>
+      <c r="J79" s="98"/>
+      <c r="K79" s="98"/>
+      <c r="L79" s="98"/>
+      <c r="M79" s="98"/>
+      <c r="N79" s="98"/>
+      <c r="O79" s="98"/>
+      <c r="P79" s="98"/>
+      <c r="Q79" s="98"/>
+      <c r="R79" s="98"/>
+      <c r="S79" s="98"/>
+      <c r="T79" s="98"/>
+      <c r="U79" s="98"/>
+      <c r="V79" s="98"/>
+      <c r="W79" s="98"/>
+      <c r="X79" s="98"/>
+      <c r="Y79" s="98"/>
+      <c r="Z79" s="98"/>
+      <c r="AA79" s="98"/>
+      <c r="AB79" s="98"/>
+      <c r="AC79" s="98"/>
+      <c r="AD79" s="98"/>
+      <c r="AE79" s="98"/>
+      <c r="AF79" s="98"/>
+      <c r="AG79" s="98"/>
+      <c r="AH79" s="98"/>
+      <c r="AI79" s="98"/>
+      <c r="AJ79" s="98"/>
+      <c r="AK79" s="98"/>
+      <c r="AL79" s="98"/>
+      <c r="AM79" s="98"/>
+      <c r="AN79" s="98"/>
+      <c r="AO79" s="98"/>
+      <c r="AP79" s="98"/>
+      <c r="AQ79" s="98"/>
+      <c r="AR79" s="98"/>
+      <c r="AS79" s="98"/>
+      <c r="AT79" s="98"/>
+      <c r="AU79" s="98"/>
+      <c r="AV79" s="98"/>
+      <c r="AW79" s="98"/>
+      <c r="AX79" s="98"/>
+      <c r="AY79" s="98"/>
+      <c r="AZ79" s="98"/>
+      <c r="BA79" s="98"/>
+      <c r="BB79" s="98"/>
+      <c r="BC79" s="98"/>
+    </row>
+    <row r="94" spans="55:55" x14ac:dyDescent="0.4">
       <c r="BC94" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="D16:E16"/>
     <mergeCell ref="D78:BC79"/>
     <mergeCell ref="F16:BC16"/>
     <mergeCell ref="F33:BC33"/>
@@ -7883,8 +8045,14 @@
     <mergeCell ref="F47:BC47"/>
     <mergeCell ref="F61:BC61"/>
     <mergeCell ref="F77:BC77"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E15 E18:E32 E35:E46 F47 E49:E60 E63:E76">
+  <conditionalFormatting sqref="E18:E32 E35:E46 F47 E49:E60 E63:E76 E3:E15">
     <cfRule type="cellIs" dxfId="6" priority="600" operator="equal">
       <formula>$J$1</formula>
     </cfRule>
@@ -7895,7 +8063,7 @@
       <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:BC15 F18:BC32 F35:BC46 F49:BC60 F63:BC76">
+  <conditionalFormatting sqref="F18:BC32 F35:BC46 F49:BC60 F63:BC76 F13:BC15">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$K$1</formula>
     </cfRule>
@@ -7910,7 +8078,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E15 E18:E32 E49:E60 E35:E45 E63:E76 F47" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F47 E18:E32 E49:E60 E35:E45 E63:E76 E3:E15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$H$1:$J$1</formula1>
     </dataValidation>
   </dataValidations>
@@ -7924,21 +8092,21 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.69140625" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.3046875" customWidth="1"/>
+    <col min="12" max="12" width="11.69140625" customWidth="1"/>
+    <col min="13" max="13" width="12.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.9" x14ac:dyDescent="0.45">
       <c r="B1" s="16" t="s">
         <v>19</v>
       </c>
@@ -7964,7 +8132,7 @@
       <c r="L1" s="42"/>
       <c r="M1" s="42"/>
     </row>
-    <row r="2" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
@@ -7972,29 +8140,29 @@
         <v>21</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
@@ -8022,9 +8190,9 @@
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B4" s="26">
         <f>SUMIF(C4:L4,A$12,C$3:Z$3)</f>
@@ -8056,9 +8224,9 @@
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B5" s="10">
         <f>SUMIF(C5:L5,A$12,C$3:Z$3)</f>
@@ -8086,9 +8254,9 @@
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B6" s="10">
         <f>SUMIF(C6:L6,A$12,C$3:Z$3)</f>
@@ -8118,9 +8286,9 @@
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B7" s="10">
         <f>SUMIF(C7:L7,A$12,C$3:Z$3)</f>
@@ -8150,9 +8318,9 @@
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B8" s="10">
         <f>SUMIF(C8:L8,A$12,C$3:Z$3)</f>
@@ -8184,7 +8352,7 @@
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
@@ -8237,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -8252,25 +8420,25 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.53515625" customWidth="1"/>
+    <col min="3" max="3" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="6"/>
       <c r="B1" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="80" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="7">
@@ -8319,92 +8487,105 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="85" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A2" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="84"/>
+      <c r="C2" s="46">
+        <v>2</v>
+      </c>
+      <c r="D2" s="81">
+        <v>4</v>
+      </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
       <c r="S2" s="44"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="107"/>
-      <c r="B3" s="86" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A3" s="104"/>
+      <c r="B3" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="63"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="47">
+        <v>2</v>
+      </c>
+      <c r="D3" s="63">
+        <v>4</v>
+      </c>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
       <c r="S3" s="44"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="107"/>
-      <c r="B4" s="86" t="s">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="104"/>
+      <c r="B4" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="63"/>
+      <c r="C4" s="47">
+        <v>3</v>
+      </c>
+      <c r="D4" s="63">
+        <v>2</v>
+      </c>
       <c r="J4" s="37"/>
-      <c r="L4" s="30"/>
       <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
       <c r="S4" s="44"/>
     </row>
-    <row r="5" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108"/>
-      <c r="B5" s="87" t="s">
+    <row r="5" spans="1:19" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="105"/>
+      <c r="B5" s="84" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="64">
         <f>SUM(C2:C4)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D5" s="65">
         <f>SUM(D2:D4)</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="113"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102"/>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="114"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="106" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="110"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="96"/>
+      <c r="S5" s="111"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A6" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="46">
         <v>4</v>
       </c>
-      <c r="D6" s="84">
+      <c r="D6" s="81">
         <v>1</v>
       </c>
       <c r="S6" s="44"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="86" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A7" s="104"/>
+      <c r="B7" s="83" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="47">
@@ -8416,9 +8597,9 @@
       <c r="J7" s="36"/>
       <c r="S7" s="44"/>
     </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="107"/>
-      <c r="B8" s="86" t="s">
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="104"/>
+      <c r="B8" s="83" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="47">
@@ -8430,9 +8611,9 @@
       <c r="J8" s="37"/>
       <c r="S8" s="44"/>
     </row>
-    <row r="9" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="108"/>
-      <c r="B9" s="87" t="s">
+    <row r="9" spans="1:19" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="105"/>
+      <c r="B9" s="84" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="64">
@@ -8443,37 +8624,37 @@
         <f>SUM(D6:D8)</f>
         <v>5</v>
       </c>
-      <c r="E9" s="113"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="102"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="114"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="106" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="85" t="s">
+      <c r="E9" s="110"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="96"/>
+      <c r="S9" s="111"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A10" s="103" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="46"/>
-      <c r="D10" s="84"/>
+      <c r="D10" s="81"/>
       <c r="E10" s="29"/>
       <c r="S10" s="44"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
-      <c r="B11" s="86" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A11" s="104"/>
+      <c r="B11" s="83" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="47"/>
@@ -8486,9 +8667,9 @@
       <c r="K11" s="30"/>
       <c r="S11" s="44"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="107"/>
-      <c r="B12" s="86" t="s">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="104"/>
+      <c r="B12" s="83" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="47"/>
@@ -8497,9 +8678,9 @@
       <c r="L12" s="30"/>
       <c r="S12" s="44"/>
     </row>
-    <row r="13" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108"/>
-      <c r="B13" s="88" t="s">
+    <row r="13" spans="1:19" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="105"/>
+      <c r="B13" s="85" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="64">
@@ -8510,38 +8691,38 @@
         <f>SUM(D10:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="113"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="102"/>
-      <c r="S13" s="114"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="106" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="85" t="s">
+      <c r="E13" s="110"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="96"/>
+      <c r="O13" s="96"/>
+      <c r="P13" s="96"/>
+      <c r="Q13" s="96"/>
+      <c r="R13" s="96"/>
+      <c r="S13" s="111"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A14" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="46"/>
-      <c r="D14" s="84"/>
+      <c r="D14" s="81"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="S14" s="44"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
-      <c r="B15" s="86" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A15" s="104"/>
+      <c r="B15" s="83" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="47"/>
@@ -8553,9 +8734,9 @@
       <c r="K15" s="30"/>
       <c r="S15" s="44"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="107"/>
-      <c r="B16" s="86" t="s">
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="104"/>
+      <c r="B16" s="83" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="47"/>
@@ -8565,9 +8746,9 @@
       <c r="M16" s="29"/>
       <c r="S16" s="44"/>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="108"/>
-      <c r="B17" s="88" t="s">
+    <row r="17" spans="1:19" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="105"/>
+      <c r="B17" s="85" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="64">
@@ -8578,39 +8759,39 @@
         <f>SUM(D14:D16)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="113"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="102"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="114"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="106" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="85" t="s">
+      <c r="E17" s="110"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="96"/>
+      <c r="S17" s="111"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A18" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="46"/>
-      <c r="D18" s="84"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="61"/>
       <c r="S18" s="44"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
-      <c r="B19" s="86" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A19" s="104"/>
+      <c r="B19" s="83" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="47"/>
@@ -8622,9 +8803,9 @@
       <c r="L19" s="29"/>
       <c r="S19" s="44"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="108"/>
-      <c r="B20" s="87" t="s">
+    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="105"/>
+      <c r="B20" s="84" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="47"/>
@@ -8633,65 +8814,65 @@
       <c r="M20" s="29"/>
       <c r="S20" s="44"/>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="111" t="s">
+    <row r="21" spans="1:19" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="112"/>
-      <c r="C21" s="89">
+      <c r="B21" s="109"/>
+      <c r="C21" s="86">
         <f>SUM(C18:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="90">
+      <c r="D21" s="87">
         <f>SUM(D18:D20)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="98"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="99"/>
-      <c r="M21" s="99"/>
-      <c r="N21" s="99"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="99"/>
-      <c r="Q21" s="99"/>
-      <c r="R21" s="99"/>
-      <c r="S21" s="115"/>
-    </row>
-    <row r="22" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="109" t="s">
+      <c r="E21" s="99"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="100"/>
+      <c r="O21" s="100"/>
+      <c r="P21" s="100"/>
+      <c r="Q21" s="100"/>
+      <c r="R21" s="100"/>
+      <c r="S21" s="112"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="110"/>
+      <c r="B22" s="107"/>
       <c r="C22" s="64">
         <f>SUM(C5,C9,C13,C17,C21)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D22" s="65">
         <f>SUM(D5,D9,D13,D17,D21)</f>
-        <v>5</v>
-      </c>
-      <c r="E22" s="116"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="117"/>
-      <c r="L22" s="117"/>
-      <c r="M22" s="117"/>
-      <c r="N22" s="117"/>
-      <c r="O22" s="117"/>
-      <c r="P22" s="117"/>
-      <c r="Q22" s="117"/>
-      <c r="R22" s="117"/>
-      <c r="S22" s="118"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E22" s="113"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="114"/>
+      <c r="J22" s="114"/>
+      <c r="K22" s="114"/>
+      <c r="L22" s="114"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="114"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="114"/>
+      <c r="Q22" s="114"/>
+      <c r="R22" s="114"/>
+      <c r="S22" s="115"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B23" s="8"/>
     </row>
   </sheetData>
@@ -8717,46 +8898,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" customWidth="1"/>
+    <col min="1" max="1" width="63.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
       <c r="B1" s="32" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="28">
-        <f>(SA!$D5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="28">
         <f>(SA!$D9)</f>
@@ -8773,21 +8949,15 @@
         <f>(SA!$D21)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="28" t="e">
-        <f>(SA!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H2" s="28" t="e">
-        <f>(SA!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28">
@@ -8799,19 +8969,15 @@
       <c r="F3" s="28">
         <v>6</v>
       </c>
-      <c r="G3" s="28">
-        <v>4</v>
-      </c>
-      <c r="H3" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="28">
@@ -8823,14 +8989,10 @@
       <c r="F4" s="28">
         <v>6</v>
       </c>
-      <c r="G4" s="28">
-        <v>7</v>
-      </c>
-      <c r="H4" s="28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
@@ -8845,14 +9007,10 @@
       <c r="F5" s="28">
         <v>4</v>
       </c>
-      <c r="G5" s="28">
-        <v>4</v>
-      </c>
-      <c r="H5" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
@@ -8866,13 +9024,13 @@
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A7" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="34">
         <f t="shared" ref="B7:H7" si="0">SUM(B2:B6)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="34">
         <f t="shared" si="0"/>
@@ -8890,14 +9048,8 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G7" s="34" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="H7" s="34" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>